<commit_message>
fix new button name + cleanup
</commit_message>
<xml_diff>
--- a/Project Outputs for Main_arduino_PCB/Main_arduino_PCB.xlsx
+++ b/Project Outputs for Main_arduino_PCB/Main_arduino_PCB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itaym\Documents\limudim\formula\main_arduino_PCB\Main_arduino_PCB\Project Outputs for Main_arduino_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BCA4AFB-3E95-4A6B-B917-B068BA4E8B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1923FD4D-656C-4DEB-847E-E2A6C763B725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7815" xr2:uid="{8DC65118-79B4-4B5D-9AF8-24D64A91A621}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="23040" windowHeight="12204" xr2:uid="{BB96F89F-5538-4596-8F26-42736508D318}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_arduino_PCB" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
   <si>
     <t>Line #</t>
   </si>
@@ -161,48 +161,24 @@
     <t>1440054-ND</t>
   </si>
   <si>
-    <t>416131160808</t>
-  </si>
-  <si>
-    <t>Slide Dip Switch, 8 Switches, SPST, Latched, 0.025A, 24VDC, 0 PCB Hole Cnt, Solder Terminal, Surface Mount-straight</t>
-  </si>
-  <si>
-    <t>counter/direct switch</t>
-  </si>
-  <si>
-    <t>CMP-00006-1</t>
-  </si>
-  <si>
-    <t>732-416131160808CT-ND</t>
-  </si>
-  <si>
-    <t>SN74LS93N</t>
-  </si>
-  <si>
-    <t>Binary Counter, LS Series, Asynchronous, Negative Edge Triggered, 3-Bit, Up Direction, TTL, PDIP14</t>
-  </si>
-  <si>
-    <t>counterBL, counterBR, counterFL, counterFR</t>
-  </si>
-  <si>
-    <t>CMP-00007-1</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>Heisener</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>I2C CAN_MODULE</t>
+    <t>MXL83411E-ADA-R</t>
+  </si>
+  <si>
+    <t>Integrated Circuit</t>
+  </si>
+  <si>
+    <t>ENC_Rx_BCK, ENC_Rx_FWD</t>
   </si>
   <si>
     <t>Not managed</t>
   </si>
   <si>
+    <t>I2C_CAN</t>
+  </si>
+  <si>
+    <t>CMP-007-000000-2</t>
+  </si>
+  <si>
     <t>A000005</t>
   </si>
   <si>
@@ -224,7 +200,10 @@
     <t>Unknown</t>
   </si>
   <si>
-    <t>13T9275</t>
+    <t>Farnell</t>
+  </si>
+  <si>
+    <t>1848691</t>
   </si>
   <si>
     <t>DFR0299</t>
@@ -243,6 +222,27 @@
   </si>
   <si>
     <t>1738-1041-ND</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF1200V</t>
+  </si>
+  <si>
+    <t>Chip Resistor, 120 Ohm, +/- 1%, 0.1 W, -55 to 155 degC, 0603 (1608 Metric), RoHS, Tape and Reel</t>
+  </si>
+  <si>
+    <t>R0, R1, R2, R3, R4, R5, R6, R7</t>
+  </si>
+  <si>
+    <t>CMP-2000-00213-2</t>
+  </si>
+  <si>
+    <t>Released</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>64R5313</t>
   </si>
 </sst>
 </file>
@@ -253,7 +253,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -333,39 +333,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -417,7 +417,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -528,6 +528,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -536,13 +543,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -607,61 +607,41 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99700E8B-3C7D-4B1D-8288-352A4FD6F86D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAC33CD-2EE1-4CEE-8334-4953C3347C8A}">
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" customWidth="1"/>
-    <col min="11" max="11" width="24" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="13" max="13" width="23.140625" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="11" max="11" width="23.109375" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="14" max="14" width="20.109375" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -708,7 +688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -755,7 +735,7 @@
         <v>10.59</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -800,7 +780,7 @@
         <v>5.16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -847,7 +827,7 @@
         <v>24.93</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -860,55 +840,33 @@
       <c r="D5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="G5" s="1"/>
       <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N5" s="1">
-        <v>6.8</v>
-      </c>
-      <c r="O5" s="1">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>20</v>
@@ -917,78 +875,84 @@
         <v>21</v>
       </c>
       <c r="H6" s="1">
-        <v>4</v>
-      </c>
-      <c r="I6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N6" s="1">
-        <v>2.97</v>
-      </c>
-      <c r="O6" s="1">
-        <v>11.87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="H7" s="1">
         <v>1</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
+      <c r="I7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" s="1">
+        <v>23.11</v>
+      </c>
+      <c r="O7" s="1">
+        <v>23.11</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
@@ -997,69 +961,69 @@
         <v>59</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="N8" s="1">
-        <v>23.23</v>
+        <v>5.9</v>
       </c>
       <c r="O8" s="1">
-        <v>23.23</v>
+        <v>5.9</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H9" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>66</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>67</v>
       </c>
       <c r="N9" s="1">
-        <v>5.9</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="O9" s="1">
-        <v>5.9</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>